<commit_message>
Correction to deal with nuclear in CES
</commit_message>
<xml_diff>
--- a/InputData/elec/BDPbES/BAU Dispatch Priority by Elec Source.xlsx
+++ b/InputData/elec/BDPbES/BAU Dispatch Priority by Elec Source.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\elec\BDPbES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-minnesota\InputData\elec\BDPbES\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="22995" windowHeight="11055"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="22995" windowHeight="11055" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -450,41 +450,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -502,15 +502,17 @@
   </sheetPr>
   <dimension ref="A1:AK17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.73046875" customWidth="1"/>
+    <col min="2" max="2" width="10.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -623,7 +625,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -771,7 +773,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -919,7 +921,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1067,895 +1069,895 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AA5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AC5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AD5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AF5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AG5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AI5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AJ5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AK5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>18</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AA6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AC6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AD6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AF6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AG6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AI6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AJ6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AK6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AA7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AC7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AD7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AF7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AG7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AI7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AJ7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AK7">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AA8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AC8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AD8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AF8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AG8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AI8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AJ8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AK8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AA9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AC9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AD9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AF9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AG9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AI9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AJ9">
         <f t="shared" ref="D9:AK17" si="2">$B9</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AK9">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AA10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AC10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AD10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AF10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AG10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AI10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AJ10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AK10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2103,7 +2105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2251,7 +2253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -2399,155 +2401,155 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>19</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14">
         <f>$B14</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AA14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AC14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AD14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AF14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AG14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AI14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AJ14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AK14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -2695,7 +2697,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -2843,7 +2845,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>22</v>
       </c>

</xml_diff>